<commit_message>
fix version on translation master file
</commit_message>
<xml_diff>
--- a/wifi4eu-scripts/src/translations/xlsx2json/Translations_Master_File-v1.15.19.xlsx
+++ b/wifi4eu-scripts/src/translations/xlsx2json/Translations_Master_File-v1.15.19.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7320"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7320" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Labels" sheetId="1" r:id="rId1"/>
@@ -99,7 +99,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12849" uniqueCount="8421">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12853" uniqueCount="8424">
   <si>
     <t>Labels</t>
   </si>
@@ -26239,6 +26239,15 @@
   </si>
   <si>
     <t>1.14.19</t>
+  </si>
+  <si>
+    <t>shared.documentsUploaded</t>
+  </si>
+  <si>
+    <t>Documents added on {{date}} at {{hour}}</t>
+  </si>
+  <si>
+    <t>1.15.19</t>
   </si>
 </sst>
 </file>
@@ -26382,7 +26391,7 @@
       <family val="3"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -26433,12 +26442,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -26575,17 +26578,177 @@
     <xf numFmtId="0" fontId="21" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Buena" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2"/>
   </cellStyles>
-  <dxfs count="87">
+  <dxfs count="103">
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -27757,13 +27920,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:AA533"/>
+  <dimension ref="A1:AA534"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D502" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B533" sqref="B533"/>
+      <selection pane="bottomRight" activeCell="M549" sqref="M548:M549"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="26.28515625" defaultRowHeight="15"/>
@@ -27890,7 +28053,7 @@
       </c>
       <c r="I2" s="6">
         <f t="shared" si="0"/>
-        <v>531</v>
+        <v>532</v>
       </c>
       <c r="J2" s="6">
         <f t="shared" si="0"/>
@@ -69831,7 +69994,7 @@
         <v>8080</v>
       </c>
       <c r="C520" s="6">
-        <f t="shared" ref="C520:C533" si="11">COUNTA(D520:ZC520)</f>
+        <f t="shared" ref="C520:C534" si="11">COUNTA(D520:ZC520)</f>
         <v>24</v>
       </c>
       <c r="D520" s="7" t="s">
@@ -70241,7 +70404,7 @@
         <v>8378</v>
       </c>
     </row>
-    <row r="528" spans="1:27" s="70" customFormat="1">
+    <row r="528" spans="1:27" s="67" customFormat="1">
       <c r="A528" s="44">
         <v>565</v>
       </c>
@@ -70279,7 +70442,7 @@
       <c r="Z528" s="51"/>
       <c r="AA528" s="51"/>
     </row>
-    <row r="529" spans="1:27" s="70" customFormat="1">
+    <row r="529" spans="1:27" s="67" customFormat="1">
       <c r="A529" s="44">
         <v>566</v>
       </c>
@@ -70317,7 +70480,7 @@
       <c r="Z529" s="51"/>
       <c r="AA529" s="51"/>
     </row>
-    <row r="530" spans="1:27" s="70" customFormat="1">
+    <row r="530" spans="1:27" s="67" customFormat="1" ht="14.25" customHeight="1">
       <c r="A530" s="44">
         <v>567</v>
       </c>
@@ -70355,7 +70518,7 @@
       <c r="Z530" s="51"/>
       <c r="AA530" s="51"/>
     </row>
-    <row r="531" spans="1:27" s="70" customFormat="1">
+    <row r="531" spans="1:27" s="67" customFormat="1">
       <c r="A531" s="44">
         <v>568</v>
       </c>
@@ -70393,7 +70556,7 @@
       <c r="Z531" s="51"/>
       <c r="AA531" s="51"/>
     </row>
-    <row r="532" spans="1:27" s="70" customFormat="1">
+    <row r="532" spans="1:27" s="67" customFormat="1" ht="15.75" customHeight="1">
       <c r="A532" s="44">
         <v>569</v>
       </c>
@@ -70431,433 +70594,524 @@
       <c r="Z532" s="51"/>
       <c r="AA532" s="51"/>
     </row>
-    <row r="533" spans="1:27">
-      <c r="A533" s="67">
+    <row r="533" spans="1:27" s="67" customFormat="1">
+      <c r="A533" s="44">
         <v>570</v>
       </c>
-      <c r="B533" s="68" t="s">
+      <c r="B533" s="60" t="s">
         <v>8419</v>
       </c>
-      <c r="C533" s="67">
+      <c r="C533" s="44">
         <f t="shared" si="11"/>
         <v>1</v>
       </c>
-      <c r="I533" s="69" t="s">
+      <c r="D533" s="51"/>
+      <c r="E533" s="51"/>
+      <c r="F533" s="51"/>
+      <c r="G533" s="51"/>
+      <c r="H533" s="51"/>
+      <c r="I533" s="51" t="s">
         <v>8418</v>
       </c>
+      <c r="J533" s="51"/>
+      <c r="K533" s="51"/>
+      <c r="L533" s="51"/>
+      <c r="M533" s="51"/>
+      <c r="N533" s="51"/>
+      <c r="O533" s="51"/>
+      <c r="P533" s="51"/>
+      <c r="Q533" s="51"/>
+      <c r="R533" s="51"/>
+      <c r="S533" s="51"/>
+      <c r="T533" s="51"/>
+      <c r="U533" s="51"/>
+      <c r="V533" s="51"/>
+      <c r="W533" s="51"/>
+      <c r="X533" s="51"/>
+      <c r="Y533" s="51"/>
+      <c r="Z533" s="51"/>
+      <c r="AA533" s="51"/>
+    </row>
+    <row r="534" spans="1:27">
+      <c r="A534" s="68">
+        <v>571</v>
+      </c>
+      <c r="B534" s="69" t="s">
+        <v>8421</v>
+      </c>
+      <c r="C534" s="6">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+      <c r="D534" s="7"/>
+      <c r="E534" s="7"/>
+      <c r="F534" s="7"/>
+      <c r="G534" s="7"/>
+      <c r="H534" s="7"/>
+      <c r="I534" s="70" t="s">
+        <v>8422</v>
+      </c>
+      <c r="J534" s="7"/>
+      <c r="K534" s="7"/>
+      <c r="L534" s="7"/>
+      <c r="M534" s="7"/>
+      <c r="N534" s="7"/>
+      <c r="O534" s="7"/>
+      <c r="P534" s="7"/>
+      <c r="Q534" s="7"/>
+      <c r="R534" s="7"/>
+      <c r="S534" s="7"/>
+      <c r="T534" s="7"/>
+      <c r="U534" s="7"/>
+      <c r="V534" s="7"/>
+      <c r="W534" s="7"/>
+      <c r="X534" s="7"/>
+      <c r="Y534" s="7"/>
+      <c r="Z534" s="7"/>
+      <c r="AA534" s="7"/>
     </row>
   </sheetData>
   <sortState ref="A2:AA522">
     <sortCondition ref="A2:A522"/>
   </sortState>
   <conditionalFormatting sqref="B509:B515 B2:B434 B504:B507 B523:B527 B536:B2954">
-    <cfRule type="beginsWith" dxfId="86" priority="138" operator="beginsWith" text="int.">
+    <cfRule type="beginsWith" dxfId="102" priority="145" operator="beginsWith" text="int.">
       <formula>LEFT(B2,4)="int."</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C2:C434 C504:C515 C522:C2954">
-    <cfRule type="cellIs" dxfId="85" priority="137" operator="lessThan">
+  <conditionalFormatting sqref="C2:C434 C504:C515 C522:C532 C535:C2954">
+    <cfRule type="cellIs" dxfId="101" priority="144" operator="lessThan">
       <formula>24</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="V16:Z16 V141:W143 Y141:AA143 X142 D330:H331 E324:H329 D333:H349 I333:AA341 I331:AA331 I346:I349 D357:AA359 J346:AA355 D351:I355 V17:AA48 U197:U203 V144:AA203 V2:AA15 D2:U35 D361:AA366 I360 P360 D368:AA409 L367 D512:AA515 D511:P511 R511:AA511 W367 O367 I367 F367 J205:T205 D206:T213 E205:H205 Q367 D50:AA92 U205:AA213 D94:T135 U94:U173 V94:AA135 D523:AA526 D504:AA510 I262:AA329 D262:H323 D215:AA261 D37:U37 D36:K36 M36:U36 D41:U48 D38:K40 M38:U40 L38:L39 D137:T203 F136:G136 J136:M136 O136 Q136 V137:AA140 V136:W136 Y136:Z136 S136:T136 D414:AA434 D410:H413 J410:AA413 D534:AA2954 D528:H533 J528:AA533">
-    <cfRule type="containsBlanks" dxfId="84" priority="135">
+  <conditionalFormatting sqref="V16:Z16 V141:W143 Y141:AA143 X142 D330:H331 E324:H329 D333:H349 I333:AA341 I331:AA331 I346:I349 D357:AA359 J346:AA355 D351:I355 V17:AA48 U197:U203 V144:AA203 V2:AA15 D2:U35 D361:AA366 I360 P360 D368:AA409 L367 D512:AA515 D511:P511 R511:AA511 W367 O367 I367 F367 J205:T205 D206:T213 E205:H205 Q367 D50:AA92 U205:AA213 D94:T135 U94:U173 V94:AA135 D523:AA526 D504:AA510 I262:AA329 D262:H323 D215:AA261 D37:U37 D36:K36 M36:U36 D41:U48 D38:K40 M38:U40 L38:L39 D137:T203 F136:G136 J136:M136 O136 Q136 V137:AA140 V136:W136 Y136:Z136 S136:T136 D414:AA434 D410:H413 J410:AA413 D535:AA2954 D528:H532 J528:AA532">
+    <cfRule type="containsBlanks" dxfId="100" priority="142">
       <formula>LEN(TRIM(D2))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U180 U185:U186 U192:U195 U188:U190">
-    <cfRule type="containsBlanks" dxfId="83" priority="118">
+    <cfRule type="containsBlanks" dxfId="99" priority="125">
       <formula>LEN(TRIM(U180))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B435:B440">
-    <cfRule type="beginsWith" dxfId="82" priority="110" operator="beginsWith" text="int.">
+    <cfRule type="beginsWith" dxfId="98" priority="117" operator="beginsWith" text="int.">
       <formula>LEFT(B435,4)="int."</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C435:C440">
-    <cfRule type="cellIs" dxfId="81" priority="109" operator="lessThan">
+    <cfRule type="cellIs" dxfId="97" priority="116" operator="lessThan">
       <formula>24</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D435:AA440">
-    <cfRule type="containsBlanks" dxfId="80" priority="111">
+    <cfRule type="containsBlanks" dxfId="96" priority="118">
       <formula>LEN(TRIM(D435))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B441:B444">
-    <cfRule type="beginsWith" dxfId="79" priority="107" operator="beginsWith" text="int.">
+    <cfRule type="beginsWith" dxfId="95" priority="114" operator="beginsWith" text="int.">
       <formula>LEFT(B441,4)="int."</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C441:C444">
-    <cfRule type="cellIs" dxfId="78" priority="106" operator="lessThan">
+    <cfRule type="cellIs" dxfId="94" priority="113" operator="lessThan">
       <formula>24</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D442:AA444">
-    <cfRule type="containsBlanks" dxfId="77" priority="108">
+    <cfRule type="containsBlanks" dxfId="93" priority="115">
       <formula>LEN(TRIM(D442))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B445:B502">
-    <cfRule type="beginsWith" dxfId="76" priority="104" operator="beginsWith" text="int.">
+    <cfRule type="beginsWith" dxfId="92" priority="111" operator="beginsWith" text="int.">
       <formula>LEFT(B445,4)="int."</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C445:C502">
-    <cfRule type="cellIs" dxfId="75" priority="103" operator="lessThan">
+    <cfRule type="cellIs" dxfId="91" priority="110" operator="lessThan">
       <formula>24</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D445:AA502">
-    <cfRule type="containsBlanks" dxfId="74" priority="105">
+    <cfRule type="containsBlanks" dxfId="90" priority="112">
       <formula>LEN(TRIM(D445))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B503">
-    <cfRule type="beginsWith" dxfId="73" priority="101" operator="beginsWith" text="int.">
+    <cfRule type="beginsWith" dxfId="89" priority="108" operator="beginsWith" text="int.">
       <formula>LEFT(B503,4)="int."</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C503">
-    <cfRule type="cellIs" dxfId="72" priority="100" operator="lessThan">
+    <cfRule type="cellIs" dxfId="88" priority="107" operator="lessThan">
       <formula>24</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D503:AA503">
-    <cfRule type="containsBlanks" dxfId="71" priority="102">
+    <cfRule type="containsBlanks" dxfId="87" priority="109">
       <formula>LEN(TRIM(D503))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U174">
-    <cfRule type="containsBlanks" dxfId="70" priority="99">
+    <cfRule type="containsBlanks" dxfId="86" priority="106">
       <formula>LEN(TRIM(U174))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U175">
-    <cfRule type="containsBlanks" dxfId="69" priority="98">
+    <cfRule type="containsBlanks" dxfId="85" priority="105">
       <formula>LEN(TRIM(U175))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U177">
-    <cfRule type="containsBlanks" dxfId="68" priority="97">
+    <cfRule type="containsBlanks" dxfId="84" priority="104">
       <formula>LEN(TRIM(U177))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U178">
-    <cfRule type="containsBlanks" dxfId="67" priority="96">
+    <cfRule type="containsBlanks" dxfId="83" priority="103">
       <formula>LEN(TRIM(U178))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U179">
-    <cfRule type="containsBlanks" dxfId="66" priority="95">
+    <cfRule type="containsBlanks" dxfId="82" priority="102">
       <formula>LEN(TRIM(U179))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U181">
-    <cfRule type="containsBlanks" dxfId="65" priority="94">
+    <cfRule type="containsBlanks" dxfId="81" priority="101">
       <formula>LEN(TRIM(U181))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U182">
-    <cfRule type="containsBlanks" dxfId="64" priority="93">
+    <cfRule type="containsBlanks" dxfId="80" priority="100">
       <formula>LEN(TRIM(U182))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U183">
-    <cfRule type="containsBlanks" dxfId="63" priority="92">
+    <cfRule type="containsBlanks" dxfId="79" priority="99">
       <formula>LEN(TRIM(U183))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U184">
-    <cfRule type="containsBlanks" dxfId="62" priority="91">
+    <cfRule type="containsBlanks" dxfId="78" priority="98">
       <formula>LEN(TRIM(U184))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U191">
-    <cfRule type="containsBlanks" dxfId="61" priority="90">
+    <cfRule type="containsBlanks" dxfId="77" priority="97">
       <formula>LEN(TRIM(U191))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U187">
-    <cfRule type="containsBlanks" dxfId="60" priority="89">
+    <cfRule type="containsBlanks" dxfId="76" priority="96">
       <formula>LEN(TRIM(U187))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U196">
-    <cfRule type="containsBlanks" dxfId="59" priority="88">
+    <cfRule type="containsBlanks" dxfId="75" priority="95">
       <formula>LEN(TRIM(U196))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D332:AA332">
-    <cfRule type="containsBlanks" dxfId="58" priority="86">
+    <cfRule type="containsBlanks" dxfId="74" priority="93">
       <formula>LEN(TRIM(D332))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I330:T330 V330:AA330">
-    <cfRule type="containsBlanks" dxfId="57" priority="85">
+    <cfRule type="containsBlanks" dxfId="73" priority="92">
       <formula>LEN(TRIM(I330))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U330">
-    <cfRule type="containsBlanks" dxfId="56" priority="84">
+    <cfRule type="containsBlanks" dxfId="72" priority="91">
       <formula>LEN(TRIM(U330))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I342:AA343">
-    <cfRule type="containsBlanks" dxfId="55" priority="83">
+    <cfRule type="containsBlanks" dxfId="71" priority="90">
       <formula>LEN(TRIM(I342))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I345:AA345">
-    <cfRule type="containsBlanks" dxfId="54" priority="82">
+    <cfRule type="containsBlanks" dxfId="70" priority="89">
       <formula>LEN(TRIM(I345))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I344:AA344">
-    <cfRule type="containsBlanks" dxfId="53" priority="81">
+    <cfRule type="containsBlanks" dxfId="69" priority="88">
       <formula>LEN(TRIM(I344))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D350:I350">
-    <cfRule type="containsBlanks" dxfId="52" priority="80">
+    <cfRule type="containsBlanks" dxfId="68" priority="87">
       <formula>LEN(TRIM(D350))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U176">
-    <cfRule type="containsBlanks" dxfId="51" priority="78">
+    <cfRule type="containsBlanks" dxfId="67" priority="85">
       <formula>LEN(TRIM(U176))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D356">
-    <cfRule type="containsBlanks" dxfId="50" priority="77">
+    <cfRule type="containsBlanks" dxfId="66" priority="84">
       <formula>LEN(TRIM(D356))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E356">
-    <cfRule type="containsBlanks" dxfId="49" priority="76">
+    <cfRule type="containsBlanks" dxfId="65" priority="83">
       <formula>LEN(TRIM(E356))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F356">
-    <cfRule type="containsBlanks" dxfId="48" priority="75">
+    <cfRule type="containsBlanks" dxfId="64" priority="82">
       <formula>LEN(TRIM(F356))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G356">
-    <cfRule type="containsBlanks" dxfId="47" priority="74">
+    <cfRule type="containsBlanks" dxfId="63" priority="81">
       <formula>LEN(TRIM(G356))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H356">
-    <cfRule type="containsBlanks" dxfId="46" priority="73">
+    <cfRule type="containsBlanks" dxfId="62" priority="80">
       <formula>LEN(TRIM(H356))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I356">
-    <cfRule type="containsBlanks" dxfId="45" priority="72">
+    <cfRule type="containsBlanks" dxfId="61" priority="79">
       <formula>LEN(TRIM(I356))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J356">
-    <cfRule type="containsBlanks" dxfId="44" priority="71">
+    <cfRule type="containsBlanks" dxfId="60" priority="78">
       <formula>LEN(TRIM(J356))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K356">
-    <cfRule type="containsBlanks" dxfId="43" priority="70">
+    <cfRule type="containsBlanks" dxfId="59" priority="77">
       <formula>LEN(TRIM(K356))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L356">
-    <cfRule type="containsBlanks" dxfId="42" priority="69">
+    <cfRule type="containsBlanks" dxfId="58" priority="76">
       <formula>LEN(TRIM(L356))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M356">
-    <cfRule type="containsBlanks" dxfId="41" priority="68">
+    <cfRule type="containsBlanks" dxfId="57" priority="75">
       <formula>LEN(TRIM(M356))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N356">
-    <cfRule type="containsBlanks" dxfId="40" priority="67">
+    <cfRule type="containsBlanks" dxfId="56" priority="74">
       <formula>LEN(TRIM(N356))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O356">
-    <cfRule type="containsBlanks" dxfId="39" priority="66">
+    <cfRule type="containsBlanks" dxfId="55" priority="73">
       <formula>LEN(TRIM(O356))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P356">
-    <cfRule type="containsBlanks" dxfId="38" priority="65">
+    <cfRule type="containsBlanks" dxfId="54" priority="72">
       <formula>LEN(TRIM(P356))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q356">
-    <cfRule type="containsBlanks" dxfId="37" priority="64">
+    <cfRule type="containsBlanks" dxfId="53" priority="71">
       <formula>LEN(TRIM(Q356))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R356">
-    <cfRule type="containsBlanks" dxfId="36" priority="63">
+    <cfRule type="containsBlanks" dxfId="52" priority="70">
       <formula>LEN(TRIM(R356))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S356">
-    <cfRule type="containsBlanks" dxfId="35" priority="62">
+    <cfRule type="containsBlanks" dxfId="51" priority="69">
       <formula>LEN(TRIM(S356))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T356">
-    <cfRule type="containsBlanks" dxfId="34" priority="61">
+    <cfRule type="containsBlanks" dxfId="50" priority="68">
       <formula>LEN(TRIM(T356))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U356">
-    <cfRule type="containsBlanks" dxfId="33" priority="60">
+    <cfRule type="containsBlanks" dxfId="49" priority="67">
       <formula>LEN(TRIM(U356))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V356">
-    <cfRule type="containsBlanks" dxfId="32" priority="59">
+    <cfRule type="containsBlanks" dxfId="48" priority="66">
       <formula>LEN(TRIM(V356))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W356">
-    <cfRule type="containsBlanks" dxfId="31" priority="58">
+    <cfRule type="containsBlanks" dxfId="47" priority="65">
       <formula>LEN(TRIM(W356))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X356">
-    <cfRule type="containsBlanks" dxfId="30" priority="57">
+    <cfRule type="containsBlanks" dxfId="46" priority="64">
       <formula>LEN(TRIM(X356))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y356">
-    <cfRule type="containsBlanks" dxfId="29" priority="56">
+    <cfRule type="containsBlanks" dxfId="45" priority="63">
       <formula>LEN(TRIM(Y356))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z356">
-    <cfRule type="containsBlanks" dxfId="28" priority="55">
+    <cfRule type="containsBlanks" dxfId="44" priority="62">
       <formula>LEN(TRIM(Z356))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA356">
-    <cfRule type="containsBlanks" dxfId="27" priority="54">
+    <cfRule type="containsBlanks" dxfId="43" priority="61">
       <formula>LEN(TRIM(AA356))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D49:AA49">
-    <cfRule type="containsBlanks" dxfId="26" priority="51">
+    <cfRule type="containsBlanks" dxfId="42" priority="58">
       <formula>LEN(TRIM(D49))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C520">
-    <cfRule type="cellIs" dxfId="25" priority="42" operator="lessThan">
+    <cfRule type="cellIs" dxfId="41" priority="49" operator="lessThan">
       <formula>24</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D520:AA520">
-    <cfRule type="containsBlanks" dxfId="24" priority="41">
+    <cfRule type="containsBlanks" dxfId="40" priority="48">
       <formula>LEN(TRIM(D520))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B520">
-    <cfRule type="beginsWith" dxfId="23" priority="40" operator="beginsWith" text="int.">
+    <cfRule type="beginsWith" dxfId="39" priority="47" operator="beginsWith" text="int.">
       <formula>LEFT(B520,4)="int."</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B516:B519">
-    <cfRule type="beginsWith" dxfId="22" priority="38" operator="beginsWith" text="int.">
+    <cfRule type="beginsWith" dxfId="38" priority="45" operator="beginsWith" text="int.">
       <formula>LEFT(B516,4)="int."</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C516:C519">
-    <cfRule type="cellIs" dxfId="21" priority="37" operator="lessThan">
+    <cfRule type="cellIs" dxfId="37" priority="44" operator="lessThan">
       <formula>24</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D516:AA519">
-    <cfRule type="containsBlanks" dxfId="20" priority="39">
+    <cfRule type="containsBlanks" dxfId="36" priority="46">
       <formula>LEN(TRIM(D516))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B508">
-    <cfRule type="beginsWith" dxfId="19" priority="34" operator="beginsWith" text="int.">
+    <cfRule type="beginsWith" dxfId="35" priority="41" operator="beginsWith" text="int.">
       <formula>LEFT(B508,4)="int."</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B522">
-    <cfRule type="beginsWith" dxfId="18" priority="26" operator="beginsWith" text="int.">
+    <cfRule type="beginsWith" dxfId="34" priority="33" operator="beginsWith" text="int.">
       <formula>LEFT(B522,4)="int."</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D522:AA522">
-    <cfRule type="containsBlanks" dxfId="17" priority="27">
+    <cfRule type="containsBlanks" dxfId="33" priority="34">
       <formula>LEN(TRIM(D522))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L204">
-    <cfRule type="containsBlanks" dxfId="16" priority="11">
+    <cfRule type="containsBlanks" dxfId="32" priority="18">
       <formula>LEN(TRIM(L204))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F204:H204 J204:K204 M204:AA204">
-    <cfRule type="containsBlanks" dxfId="15" priority="15">
+    <cfRule type="containsBlanks" dxfId="31" priority="22">
       <formula>LEN(TRIM(F204))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I204">
-    <cfRule type="containsBlanks" dxfId="14" priority="12">
+    <cfRule type="containsBlanks" dxfId="30" priority="19">
       <formula>LEN(TRIM(I204))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D204">
-    <cfRule type="containsBlanks" dxfId="13" priority="14">
+    <cfRule type="containsBlanks" dxfId="29" priority="21">
       <formula>LEN(TRIM(D204))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E204">
-    <cfRule type="containsBlanks" dxfId="12" priority="13">
+    <cfRule type="containsBlanks" dxfId="28" priority="20">
       <formula>LEN(TRIM(E204))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D93:AA93">
-    <cfRule type="containsBlanks" dxfId="11" priority="10">
+    <cfRule type="containsBlanks" dxfId="27" priority="17">
       <formula>LEN(TRIM(D93))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D214:AA214">
-    <cfRule type="containsBlanks" dxfId="10" priority="7">
+    <cfRule type="containsBlanks" dxfId="26" priority="14">
       <formula>LEN(TRIM(D214))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D441:AA441">
-    <cfRule type="containsBlanks" dxfId="9" priority="6">
+    <cfRule type="containsBlanks" dxfId="25" priority="13">
       <formula>LEN(TRIM(D441))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I528:I532">
-    <cfRule type="containsBlanks" dxfId="8" priority="4">
+    <cfRule type="containsBlanks" dxfId="24" priority="11">
       <formula>LEN(TRIM(I528))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B528:B531">
-    <cfRule type="beginsWith" dxfId="7" priority="3" operator="beginsWith" text="int.">
+    <cfRule type="beginsWith" dxfId="23" priority="10" operator="beginsWith" text="int.">
       <formula>LEFT(B528,4)="int."</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B532:B535">
-    <cfRule type="beginsWith" dxfId="6" priority="2" operator="beginsWith" text="int.">
+  <conditionalFormatting sqref="B532 B535">
+    <cfRule type="beginsWith" dxfId="22" priority="9" operator="beginsWith" text="int.">
       <formula>LEFT(B532,4)="int."</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="C533">
+    <cfRule type="cellIs" dxfId="14" priority="7" operator="lessThan">
+      <formula>24</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D533:H533 J533:AA533">
+    <cfRule type="containsBlanks" dxfId="12" priority="6">
+      <formula>LEN(TRIM(D533))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="I533">
-    <cfRule type="containsBlanks" dxfId="5" priority="1">
+    <cfRule type="containsBlanks" dxfId="10" priority="5">
       <formula>LEN(TRIM(I533))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B533">
+    <cfRule type="beginsWith" dxfId="8" priority="4" operator="beginsWith" text="int.">
+      <formula>LEFT(B533,4)="int."</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C534">
+    <cfRule type="cellIs" dxfId="5" priority="3" operator="lessThan">
+      <formula>24</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D534:AA534">
+    <cfRule type="containsBlanks" dxfId="3" priority="2">
+      <formula>LEN(TRIM(D534))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B534">
+    <cfRule type="beginsWith" dxfId="1" priority="1" operator="beginsWith" text="int.">
+      <formula>LEFT(B534,4)="int."</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -73648,27 +73902,27 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B3">
-    <cfRule type="beginsWith" dxfId="4" priority="5" operator="beginsWith" text="int.">
+    <cfRule type="beginsWith" dxfId="20" priority="5" operator="beginsWith" text="int.">
       <formula>LEFT(B3,4)="int."</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3:C16">
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="lessThan">
+    <cfRule type="cellIs" dxfId="19" priority="4" operator="lessThan">
       <formula>24</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2">
-    <cfRule type="beginsWith" dxfId="2" priority="3" operator="beginsWith" text="int.">
+    <cfRule type="beginsWith" dxfId="18" priority="3" operator="beginsWith" text="int.">
       <formula>LEFT(B2,4)="int."</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="17" priority="2" operator="lessThan">
       <formula>24</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:AA2">
-    <cfRule type="containsBlanks" dxfId="0" priority="1">
+    <cfRule type="containsBlanks" dxfId="16" priority="1">
       <formula>LEN(TRIM(D2))=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -73681,8 +73935,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C45"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="K27" sqref="K27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.28515625" defaultRowHeight="15"/>
@@ -74032,7 +74286,15 @@
       </c>
     </row>
     <row r="32" spans="1:3">
-      <c r="B32"/>
+      <c r="A32" t="s">
+        <v>8423</v>
+      </c>
+      <c r="B32" s="45">
+        <v>43187</v>
+      </c>
+      <c r="C32" t="s">
+        <v>6499</v>
+      </c>
     </row>
     <row r="33" spans="2:2">
       <c r="B33"/>
@@ -74520,16 +74782,16 @@
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{952339DF-82CB-4830-AE94-650A16D252E0}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="6a030ef6-6c47-454f-834f-14ceab815460"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="866aabb8-7ec2-447a-a7ff-f911015037e7"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>